<commit_message>
psnr of DP and prop-table-v1 updated
</commit_message>
<xml_diff>
--- a/realsense/numbers/PSNR/ideal/psnr-average_real_ideal_nph_tileExpand.xlsx
+++ b/realsense/numbers/PSNR/ideal/psnr-average_real_ideal_nph_tileExpand.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taw11\source\repos2\At-oZ\realsense\realsense\numbers\PSNR\ideal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\渡辺　哲生\source\repos\realsense\realsense\numbers\PSNR\ideal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58973B5-93E3-4254-A341-8B41B83B004D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA34400-70BB-4324-A31F-5C8BBE6D8130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{F8221B24-CE8C-4284-B96B-48EDE3EFD3FB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" xr2:uid="{F8221B24-CE8C-4284-B96B-48EDE3EFD3FB}"/>
   </bookViews>
   <sheets>
     <sheet name="average" sheetId="1" r:id="rId1"/>
@@ -920,7 +920,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>1024mm</c:v>
+            <c:v>512mm</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -2971,9 +2971,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 テーマ">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3011,7 +3011,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3117,7 +3117,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3259,7 +3259,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3269,8 +3269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37810512-63FB-4319-992E-A5FCCE9FA93B}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="W32" sqref="W32"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="U31" sqref="U31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
psnr and speed data updated
</commit_message>
<xml_diff>
--- a/realsense/numbers/PSNR/ideal/psnr-average_real_ideal_nph_tileExpand.xlsx
+++ b/realsense/numbers/PSNR/ideal/psnr-average_real_ideal_nph_tileExpand.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taw11\source\repos2\At-oZ\realsense\realsense\numbers\PSNR\ideal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\渡辺　哲生\source\repos\realsense\realsense\numbers\PSNR\ideal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E1405F-2903-449C-B298-99AAE74BFE12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F2619F-3632-4D1B-9E1A-E09F1A0392CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{F8221B24-CE8C-4284-B96B-48EDE3EFD3FB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" xr2:uid="{F8221B24-CE8C-4284-B96B-48EDE3EFD3FB}"/>
   </bookViews>
   <sheets>
     <sheet name="average" sheetId="1" r:id="rId1"/>
@@ -728,7 +728,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12554044380816035"/>
+          <c:y val="5.8909771524461092E-2"/>
+          <c:w val="0.82376025549253895"/>
+          <c:h val="0.71445643474893505"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -1293,10 +1303,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1307,17 +1314,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="60000"/>
-                    <a:lumOff val="40000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="accent4"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -1845,7 +1846,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1860,7 +1861,7 @@
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="tx1"/>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -2189,12 +2190,7 @@
         <c:minorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="5000"/>
-                  <a:lumOff val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -2316,10 +2312,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.80769230769230771"/>
-          <c:y val="7.3529411764705885E-2"/>
-          <c:w val="0.12762237762237763"/>
-          <c:h val="0.36968992846482424"/>
+          <c:x val="0.78671328671328666"/>
+          <c:y val="0.32843137254901961"/>
+          <c:w val="0.14860139860139859"/>
+          <c:h val="0.38602979774586998"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -2339,7 +2335,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2949,14 +2945,14 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>215900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2985,9 +2981,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 テーマ">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3025,7 +3021,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3131,7 +3127,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3273,7 +3269,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3283,8 +3279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37810512-63FB-4319-992E-A5FCCE9FA93B}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="AD24" sqref="AD24"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>